<commit_message>
aanpassingen gemaakt aan de logincheck en login class
</commit_message>
<xml_diff>
--- a/logboek/logboek fotosjaak.xlsx
+++ b/logboek/logboek fotosjaak.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="39">
   <si>
     <t>Logboek</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>LoginClass zet de database values in lokale values.</t>
+  </si>
+  <si>
+    <t>loginclasstest maken met button.</t>
   </si>
   <si>
     <t>weeknr</t>
@@ -1000,7 +1003,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F14" activeCellId="0" pane="topLeft" sqref="F14"/>
+      <selection activeCell="J3" activeCellId="0" pane="topLeft" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -1062,7 +1065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>18</v>
       </c>
@@ -1072,17 +1075,27 @@
       <c r="C7" s="2" t="n">
         <v>0.604166666666667</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="n">
+        <v>0.635416666666667</v>
+      </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="G7" s="3" t="n">
         <f aca="false">(D7-C7)</f>
-        <v>-0.604166666666667</v>
+        <v>0.0312499999999996</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>41614</v>
+      </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="0" t="n">
@@ -1181,7 +1194,7 @@
       </c>
       <c r="G19" s="3" t="n">
         <f aca="false">SUM(G7:G13)</f>
-        <v>-0.604166666666667</v>
+        <v>0.0312499999999996</v>
       </c>
     </row>
   </sheetData>
@@ -1228,10 +1241,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">

</xml_diff>

<commit_message>
sessionclass gemaakt loginclass bijgewerkt
</commit_message>
<xml_diff>
--- a/logboek/logboek fotosjaak.xlsx
+++ b/logboek/logboek fotosjaak.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="141" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="5" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="141" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="week45" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,14 +13,15 @@
     <sheet name="week47" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="week48" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="week49" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="totaal" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="week50" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="totaal" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="41">
   <si>
     <t>Logboek</t>
   </si>
@@ -131,6 +132,12 @@
   </si>
   <si>
     <t>loginclasstest maken met button.</t>
+  </si>
+  <si>
+    <t>Een nieuw tabblad toegevoegd aan het logboek en</t>
+  </si>
+  <si>
+    <t>Sessionclass toegevoegd loginclass bijgewerkt</t>
   </si>
   <si>
     <t>weeknr</t>
@@ -1002,8 +1009,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="J3" activeCellId="0" pane="topLeft" sqref="J3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D9" activeCellId="0" pane="topLeft" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -1086,7 +1093,7 @@
       </c>
       <c r="G7" s="3" t="n">
         <f aca="false">(D7-C7)</f>
-        <v>0.0312499999999996</v>
+        <v>0.03125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="8">
@@ -1096,14 +1103,18 @@
       <c r="B8" s="6" t="n">
         <v>41614</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="5" t="n">
+        <v>0.40625</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.5625</v>
+      </c>
       <c r="E8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G8" s="3" t="n">
         <f aca="false">(D8-C8)</f>
-        <v>0</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
@@ -1194,7 +1205,7 @@
       </c>
       <c r="G19" s="3" t="n">
         <f aca="false">SUM(G7:G13)</f>
-        <v>0.0312499999999996</v>
+        <v>0.1875</v>
       </c>
     </row>
   </sheetData>
@@ -1213,10 +1224,230 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B9"/>
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F8" activeCellId="0" pane="topLeft" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.23979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>41613</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0.364583333333333</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0.370833333333333</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <f aca="false">(D7-C7)</f>
+        <v>0.00625000000000003</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>41614</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0.371527777777778</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <f aca="false">(D8-C8)</f>
+        <v>0.0555555555555555</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
+      <c r="B9" s="6"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="3" t="n">
+        <f aca="false">(D9-C9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="3" t="n">
+        <f aca="false">(D10-C10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="3" t="n">
+        <f aca="false">(D11-C11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="12">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <f aca="false">(D12-C12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="13">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <f aca="false">(D13-C13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="14">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="15">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F15" s="8"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="16">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" s="8"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="19">
+      <c r="F19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <f aca="false">SUM(G7:G13)</f>
+        <v>0.0618055555555556</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standaard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B10" activeCellId="0" pane="topLeft" sqref="B10"/>
+      <selection activeCell="B12" activeCellId="0" pane="topLeft" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -1241,10 +1472,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">
@@ -1266,12 +1497,34 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <f aca="false">week49!G19</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <f aca="false">week50!G19</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3" t="n">
-        <f aca="false">SUM(B7:B8)</f>
-        <v>0.200694444444444</v>
+      <c r="B11" s="3" t="n">
+        <f aca="false">SUM(B7:B10)</f>
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed login class and removed some files
</commit_message>
<xml_diff>
--- a/logboek/logboek fotosjaak.xlsx
+++ b/logboek/logboek fotosjaak.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="141" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="6" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="122" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="week45" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,14 +14,16 @@
     <sheet name="week48" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="week49" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="week50" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="totaal" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="week 2" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Toets 1 Game" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="totaal" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="65">
   <si>
     <t>Logboek</t>
   </si>
@@ -144,6 +146,72 @@
   </si>
   <si>
     <t>Sessionclass afgemaakt en logout toegevoegd.</t>
+  </si>
+  <si>
+    <t>register form aangepast aan database.</t>
+  </si>
+  <si>
+    <t>check_if_emailaddress_exists() aangemaakt in de login class</t>
+  </si>
+  <si>
+    <t>project:</t>
+  </si>
+  <si>
+    <t>Pyramid Panic</t>
+  </si>
+  <si>
+    <t>naam:</t>
+  </si>
+  <si>
+    <t>Arjan de Ruijter</t>
+  </si>
+  <si>
+    <t>afdeling:</t>
+  </si>
+  <si>
+    <t>AM1B</t>
+  </si>
+  <si>
+    <t>Toets 1 GameScenes</t>
+  </si>
+  <si>
+    <t>Maak een mapje in de solutionexplorer genaamd ScoresScene</t>
+  </si>
+  <si>
+    <t>Maak een class ScoresScene in de ScoresScene map</t>
+  </si>
+  <si>
+    <t>Pas de usings aan en maak de ScoresScene class public</t>
+  </si>
+  <si>
+    <t>Laat de class de interface implementeren IState</t>
+  </si>
+  <si>
+    <t>Kopieer de inhoud van de PlayScene class naar de ScoresScene class en verander de naam van de constructor</t>
+  </si>
+  <si>
+    <t>Maak een commit met naam: Toets1 commit 1</t>
+  </si>
+  <si>
+    <t>Maak een field scoresScene van het type ScoresScene in de PyramidPanic class</t>
+  </si>
+  <si>
+    <t>Maak een property voor het scoresScene field (een getter) in de PyramidPanic class</t>
+  </si>
+  <si>
+    <t>Controleren de namespace waar de ScoresScene class in staat. Kijk of dit ook de naam PyramidPanic draagt</t>
+  </si>
+  <si>
+    <t>Geef de achtergrondkleur in de ScoreScene class de waarde PeachPuff</t>
+  </si>
+  <si>
+    <t>Maak een nieuw object van de class ScoresScene aan in de LoadContent() method van de PyramidPanic class</t>
+  </si>
+  <si>
+    <t>Zorg dat je met het toetsenbord via de knoppen naar  ScoresScene kunt gaan</t>
+  </si>
+  <si>
+    <t>Maak een commit met naam: Toets1 commit 2</t>
   </si>
   <si>
     <t>weeknr</t>
@@ -156,15 +224,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="8">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="D\ MMMM\ YYYY" numFmtId="165"/>
     <numFmt formatCode="HH:MM" numFmtId="166"/>
     <numFmt formatCode="HH:MM:SS" numFmtId="167"/>
     <numFmt formatCode="DD/MM/YY" numFmtId="168"/>
     <numFmt formatCode="@" numFmtId="169"/>
+    <numFmt formatCode="D\ MMMM\ YYYY;@" numFmtId="170"/>
+    <numFmt formatCode="H:MM;@" numFmtId="171"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -185,6 +255,27 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -229,7 +320,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -264,6 +355,42 @@
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="171" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
@@ -1232,7 +1359,7 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="F26" activeCellId="0" pane="topLeft" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -1316,7 +1443,7 @@
       </c>
       <c r="G7" s="3" t="n">
         <f aca="false">(D7-C7)</f>
-        <v>0.00625000000000003</v>
+        <v>0.00624999999999998</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="8">
@@ -1340,7 +1467,7 @@
       </c>
       <c r="G8" s="3" t="n">
         <f aca="false">(D8-C8)</f>
-        <v>0.0555555555555555</v>
+        <v>0.055555555555555</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="9">
@@ -1359,7 +1486,7 @@
       </c>
       <c r="G9" s="3" t="n">
         <f aca="false">(D9-C9)</f>
-        <v>0.0458333333333333</v>
+        <v>0.0458333333333331</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
@@ -1377,7 +1504,7 @@
       </c>
       <c r="G10" s="3" t="n">
         <f aca="false">(D10-C10)</f>
-        <v>0.0388888888888889</v>
+        <v>0.038888888888889</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11">
@@ -1443,7 +1570,7 @@
       </c>
       <c r="G19" s="3" t="n">
         <f aca="false">SUM(G7:G13)</f>
-        <v>0.146527777777778</v>
+        <v>0.146527777777777</v>
       </c>
     </row>
   </sheetData>
@@ -1462,10 +1589,551 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B11"/>
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F8" activeCellId="0" pane="topLeft" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.23979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="56.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>41613</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0.604166666666667</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <f aca="false">(D7-C7)</f>
+        <v>0.0416666666666666</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>41614</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0.371527777777778</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <f aca="false">(D8-C8)</f>
+        <v>0.055555555555555</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
+      <c r="B9" s="6"/>
+      <c r="C9" s="2" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0.483333333333333</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="3" t="n">
+        <f aca="false">(D9-C9)</f>
+        <v>0.0458333333333331</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
+      <c r="C10" s="2" t="n">
+        <v>0.484027777777778</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0.522916666666667</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="3" t="n">
+        <f aca="false">(D10-C10)</f>
+        <v>0.038888888888889</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="3" t="n">
+        <f aca="false">(D11-C11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="12">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <f aca="false">(D12-C12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="13">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <f aca="false">(D13-C13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="14">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="15">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F15" s="8"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="16">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" s="8"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="19">
+      <c r="F19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <f aca="false">SUM(G7:G13)</f>
+        <v>0.181944444444444</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standaard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B12" activeCellId="0" pane="topLeft" sqref="B12"/>
+      <selection activeCell="A23" activeCellId="0" pane="topLeft" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="52.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="19.65" outlineLevel="0" r="1">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="2">
+      <c r="A2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.85" outlineLevel="0" r="3">
+      <c r="A3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20.85" outlineLevel="0" r="4">
+      <c r="A4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.85" outlineLevel="0" r="5"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
+      <c r="A6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.4" outlineLevel="0" r="7">
+      <c r="A7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="14" t="n">
+        <v>41628</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="15" t="n">
+        <f aca="false">D7-C7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.4" outlineLevel="0" r="8">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="15" t="n">
+        <f aca="false">D8-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21.6" outlineLevel="0" r="9">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="15" t="n">
+        <f aca="false">D9-C9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20.85" outlineLevel="0" r="10">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="15" t="n">
+        <f aca="false">D10-C10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="33.55" outlineLevel="0" r="11">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="15" t="n">
+        <f aca="false">D11-C11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="19.4" outlineLevel="0" r="12">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="13" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="15" t="n">
+        <f aca="false">D12-C12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="35.8" outlineLevel="0" r="13">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="13" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="15" t="n">
+        <f aca="false">D13-C13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.3" outlineLevel="0" r="14">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="15" t="n">
+        <f aca="false">D14-C14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="31.3" outlineLevel="0" r="15">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="13" t="n">
+        <v>9</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="15" t="n">
+        <f aca="false">D15-C15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="28.35" outlineLevel="0" r="16">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="15" t="n">
+        <f aca="false">D16-C16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36.55" outlineLevel="0" r="17">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="13" t="n">
+        <v>11</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="15" t="n">
+        <f aca="false">D17-C17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="27.6" outlineLevel="0" r="18">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="13" t="n">
+        <v>12</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="15" t="n">
+        <f aca="false">D18-C18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20.1" outlineLevel="0" r="19">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="13" t="n">
+        <v>13</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="15" t="n">
+        <f aca="false">D19-C19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="15" t="n">
+        <f aca="false">SUM(G7:G18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.85" outlineLevel="0" r="21"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.85" outlineLevel="0" r="22"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standaard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:B12"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="N16" activeCellId="0" pane="topLeft" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -1490,10 +2158,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">
@@ -1518,22 +2186,18 @@
       <c r="A9" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="3" t="n">
         <f aca="false">week49!G19</f>
-        <is>
-          <t/>
-        </is>
+        <v>0.1875</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="3" t="n">
         <f aca="false">week50!G19</f>
-        <is>
-          <t/>
-        </is>
+        <v>0.146527777777777</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11">
@@ -1542,9 +2206,10 @@
       </c>
       <c r="B11" s="3" t="n">
         <f aca="false">SUM(B7:B10)</f>
-        <v>0.534722222222222</v>
-      </c>
-    </row>
+        <v>0.534722222222221</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.85" outlineLevel="0" r="12"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>